<commit_message>
updated code to have new stock ecoogical indicators. Need to correct code to match stock-fishing country as two stocks changed the name: CONASTOR is CODNEARNWC and CODNS is now CODIIIaW
</commit_message>
<xml_diff>
--- a/data/Lat_RI_Stock.xlsx
+++ b/data/Lat_RI_Stock.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elenaojea/OneDrive/P_RESEARCH/P_RESEARCH_PUBLICATIONS/PUBLICATIONS_ONGOING/RESILIENCE INDEXELENA/Scientific Reports/Revision Scientific Reports/work ecological index/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elenaojea/OneDrive/P_RESEARCH/P_RESEARCH_PUBLICATIONS/PUBLICATIONS_ONGOING/RESILIENCE INDEXELENA/Scientific Reports/Revision Scientific Reports/RESUBMISSION SR 2020/Fisheries-Resilience-Index/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27075137-55AD-C444-98C8-CAA41B27290C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27100" windowHeight="14680"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27100" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -62,9 +63,6 @@
     <t>Atlantic cod</t>
   </si>
   <si>
-    <t>CODCOASTNOR</t>
-  </si>
-  <si>
     <t>CODNEAR</t>
   </si>
   <si>
@@ -86,13 +84,16 @@
     <t>CODVIa</t>
   </si>
   <si>
-    <t>CODNS</t>
+    <t>CODNEARNCW</t>
+  </si>
+  <si>
+    <t>CODIIIaW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -158,9 +159,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -172,7 +173,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -198,7 +198,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -262,7 +262,7 @@
                   <c:v>CODBA2532</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CODNS</c:v>
+                  <c:v>CODIIIaW</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>CODVIa</c:v>
@@ -277,7 +277,7 @@
                   <c:v>CODICE</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>CODCOASTNOR</c:v>
+                  <c:v>CODNEARNCW</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>CODNEAR</c:v>
@@ -292,31 +292,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>40.71666666666667</c:v>
+                  <c:v>40.716666666666669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53.1525198938992</c:v>
+                  <c:v>53.152519893899203</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53.5462962962963</c:v>
+                  <c:v>53.546296296296298</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.51190476190476</c:v>
+                  <c:v>56.511904761904759</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>56.94742489270386</c:v>
+                  <c:v>56.947424892703864</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>57.37650602409639</c:v>
+                  <c:v>57.376506024096386</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.96666666666667</c:v>
+                  <c:v>57.966666666666669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>61.59745762711864</c:v>
+                  <c:v>61.597457627118644</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>65.1198224852071</c:v>
+                  <c:v>65.119822485207095</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>75.38378566457898</c:v>
@@ -328,6 +328,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CC58-0E4A-9DA6-90780646EE1E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -383,7 +388,7 @@
                   <c:v>CODBA2532</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CODNS</c:v>
+                  <c:v>CODIIIaW</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>CODVIa</c:v>
@@ -398,7 +403,7 @@
                   <c:v>CODICE</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>CODCOASTNOR</c:v>
+                  <c:v>CODNEARNCW</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>CODNEAR</c:v>
@@ -449,6 +454,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CC58-0E4A-9DA6-90780646EE1E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -504,7 +514,7 @@
                   <c:v>CODBA2532</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>CODNS</c:v>
+                  <c:v>CODIIIaW</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>CODVIa</c:v>
@@ -519,7 +529,7 @@
                   <c:v>CODICE</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>CODCOASTNOR</c:v>
+                  <c:v>CODNEARNCW</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>CODNEAR</c:v>
@@ -570,6 +580,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CC58-0E4A-9DA6-90780646EE1E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -636,7 +651,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-891681568"/>
@@ -664,6 +679,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -697,7 +713,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-915466080"/>
@@ -714,7 +730,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -740,7 +755,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -770,7 +785,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1354,7 +1369,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1634,11 +1655,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1708,7 +1729,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>0.30867498969051954</v>
@@ -1728,7 +1749,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>0.48205891800891837</v>
@@ -1768,7 +1789,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>0.10714285714285714</v>
@@ -1788,7 +1809,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>0.57365316839939728</v>
@@ -1808,7 +1829,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>0.62276410560735429</v>
@@ -1828,7 +1849,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>0.46926896120402922</v>
@@ -1847,8 +1868,8 @@
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
+      <c r="B11" t="s">
+        <v>17</v>
       </c>
       <c r="C11">
         <v>0.18020502240760244</v>
@@ -1868,7 +1889,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>0.72014308832590179</v>

</xml_diff>